<commit_message>
version 3.01 description: 修改了sumsales_year下各个分类的列的前后顺序
</commit_message>
<xml_diff>
--- a/classificationFile_sales/sumSales_year/水生根茎类_sales.xlsx
+++ b/classificationFile_sales/sumSales_year/水生根茎类_sales.xlsx
@@ -16,73 +16,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
   <si>
+    <t>单品名称</t>
+  </si>
+  <si>
     <t>分类名称</t>
   </si>
   <si>
-    <t>单品名称</t>
-  </si>
-  <si>
     <t>年份</t>
   </si>
   <si>
     <t>销量(千克)</t>
   </si>
   <si>
+    <t>净藕(1)</t>
+  </si>
+  <si>
+    <t>净藕(2)</t>
+  </si>
+  <si>
+    <t>净藕(3)</t>
+  </si>
+  <si>
+    <t>洪湖莲藕(粉藕)</t>
+  </si>
+  <si>
+    <t>洪湖莲藕(脆藕)</t>
+  </si>
+  <si>
+    <t>洪湖藕带</t>
+  </si>
+  <si>
+    <t>红莲藕带</t>
+  </si>
+  <si>
+    <t>荸荠</t>
+  </si>
+  <si>
+    <t>荸荠(份)</t>
+  </si>
+  <si>
+    <t>莲蓬(个)</t>
+  </si>
+  <si>
+    <t>菱角</t>
+  </si>
+  <si>
+    <t>藕尖</t>
+  </si>
+  <si>
+    <t>野生粉藕</t>
+  </si>
+  <si>
+    <t>野藕(1)</t>
+  </si>
+  <si>
+    <t>野藕(2)</t>
+  </si>
+  <si>
+    <t>高瓜(1)</t>
+  </si>
+  <si>
+    <t>高瓜(2)</t>
+  </si>
+  <si>
+    <t>鲜藕带(袋)</t>
+  </si>
+  <si>
     <t>水生根茎类</t>
-  </si>
-  <si>
-    <t>净藕(1)</t>
-  </si>
-  <si>
-    <t>净藕(2)</t>
-  </si>
-  <si>
-    <t>净藕(3)</t>
-  </si>
-  <si>
-    <t>洪湖莲藕(粉藕)</t>
-  </si>
-  <si>
-    <t>洪湖莲藕(脆藕)</t>
-  </si>
-  <si>
-    <t>洪湖藕带</t>
-  </si>
-  <si>
-    <t>红莲藕带</t>
-  </si>
-  <si>
-    <t>荸荠</t>
-  </si>
-  <si>
-    <t>荸荠(份)</t>
-  </si>
-  <si>
-    <t>莲蓬(个)</t>
-  </si>
-  <si>
-    <t>菱角</t>
-  </si>
-  <si>
-    <t>藕尖</t>
-  </si>
-  <si>
-    <t>野生粉藕</t>
-  </si>
-  <si>
-    <t>野藕(1)</t>
-  </si>
-  <si>
-    <t>野藕(2)</t>
-  </si>
-  <si>
-    <t>高瓜(1)</t>
-  </si>
-  <si>
-    <t>高瓜(2)</t>
-  </si>
-  <si>
-    <t>鲜藕带(袋)</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>2020</v>
@@ -479,7 +479,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>2021</v>
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>2022</v>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>2023</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>2023</v>
@@ -532,10 +532,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>2022</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>2023</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>2020</v>
@@ -574,10 +574,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>2021</v>
@@ -588,10 +588,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>2022</v>
@@ -602,10 +602,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>2023</v>
@@ -616,10 +616,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>2022</v>
@@ -630,10 +630,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2020</v>
@@ -644,10 +644,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>2021</v>
@@ -658,10 +658,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>2022</v>
@@ -672,10 +672,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>2023</v>
@@ -686,10 +686,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>2020</v>
@@ -700,10 +700,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>2022</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>2023</v>
@@ -728,10 +728,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>2020</v>
@@ -742,10 +742,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>2021</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>2022</v>
@@ -770,10 +770,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>2023</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>2022</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>2020</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>2021</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C28">
         <v>2022</v>
@@ -840,10 +840,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>2020</v>
@@ -854,10 +854,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <v>2021</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>2022</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>2023</v>
@@ -896,10 +896,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>2021</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>2022</v>
@@ -924,10 +924,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>2020</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>2021</v>
@@ -952,10 +952,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C37">
         <v>2023</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>2020</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>2021</v>
@@ -994,10 +994,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>2022</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C41">
         <v>2023</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C42">
         <v>2022</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C43">
         <v>2020</v>
@@ -1050,10 +1050,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C44">
         <v>2021</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>2022</v>
@@ -1078,10 +1078,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>2023</v>
@@ -1092,10 +1092,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47">
         <v>2022</v>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C48">
         <v>2023</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
         <v>22</v>

</xml_diff>